<commit_message>
Minor fixes and changes to usable items.
</commit_message>
<xml_diff>
--- a/resources/data-imports/items-second-set.xlsx
+++ b/resources/data-imports/items-second-set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5448366F-05A4-F547-B6C7-8A08B18EE9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A855B028-1601-1A4F-9E97-16EF865EA42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1020,9 +1020,6 @@
     <t>labyrinth</t>
   </si>
   <si>
-    <t>River Stix Sandals</t>
-  </si>
-  <si>
     <t>Walk across water made to kill you.</t>
   </si>
   <si>
@@ -1360,6 +1357,9 @@
   </si>
   <si>
     <t>Purgatories Lantern</t>
+  </si>
+  <si>
+    <t>River Styx Sandals</t>
   </si>
 </sst>
 </file>
@@ -1708,8 +1708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D130" sqref="D130"/>
+    <sheetView tabSelected="1" topLeftCell="AT134" workbookViewId="0">
+      <selection activeCell="D179" sqref="D179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9979,22 +9979,22 @@
     </row>
     <row r="85" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D85" t="s">
-        <v>329</v>
+        <v>442</v>
       </c>
       <c r="E85" t="s">
         <v>301</v>
       </c>
       <c r="F85" t="s">
+        <v>329</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85">
+        <v>0</v>
+      </c>
+      <c r="X85" t="s">
         <v>330</v>
-      </c>
-      <c r="L85">
-        <v>0</v>
-      </c>
-      <c r="M85">
-        <v>0</v>
-      </c>
-      <c r="X85" t="s">
-        <v>331</v>
       </c>
       <c r="Z85">
         <v>1</v>
@@ -10050,22 +10050,22 @@
     </row>
     <row r="86" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D86" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E86" t="s">
         <v>301</v>
       </c>
       <c r="F86" t="s">
+        <v>332</v>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86">
+        <v>0</v>
+      </c>
+      <c r="X86" t="s">
         <v>333</v>
-      </c>
-      <c r="L86">
-        <v>0</v>
-      </c>
-      <c r="M86">
-        <v>0</v>
-      </c>
-      <c r="X86" t="s">
-        <v>334</v>
       </c>
       <c r="AF86">
         <v>0</v>
@@ -10118,22 +10118,22 @@
     </row>
     <row r="87" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D87" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E87" t="s">
         <v>301</v>
       </c>
       <c r="F87" t="s">
+        <v>335</v>
+      </c>
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87">
+        <v>0</v>
+      </c>
+      <c r="X87" t="s">
         <v>336</v>
-      </c>
-      <c r="L87">
-        <v>0</v>
-      </c>
-      <c r="M87">
-        <v>0</v>
-      </c>
-      <c r="X87" t="s">
-        <v>337</v>
       </c>
       <c r="AF87">
         <v>0</v>
@@ -10186,13 +10186,13 @@
     </row>
     <row r="88" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D88" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E88" t="s">
         <v>301</v>
       </c>
       <c r="F88" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="L88">
         <v>0</v>
@@ -10254,13 +10254,13 @@
     </row>
     <row r="89" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D89" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E89" t="s">
         <v>301</v>
       </c>
       <c r="F89" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L89">
         <v>0</v>
@@ -10322,25 +10322,25 @@
     </row>
     <row r="90" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D90" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E90" t="s">
         <v>301</v>
       </c>
       <c r="F90" t="s">
+        <v>342</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90">
+        <v>0</v>
+      </c>
+      <c r="Z90">
+        <v>1</v>
+      </c>
+      <c r="AD90" t="s">
         <v>343</v>
-      </c>
-      <c r="L90">
-        <v>0</v>
-      </c>
-      <c r="M90">
-        <v>0</v>
-      </c>
-      <c r="Z90">
-        <v>1</v>
-      </c>
-      <c r="AD90" t="s">
-        <v>344</v>
       </c>
       <c r="AE90">
         <v>0.5</v>
@@ -10399,25 +10399,25 @@
     </row>
     <row r="91" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D91" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E91" t="s">
         <v>301</v>
       </c>
       <c r="F91" t="s">
+        <v>345</v>
+      </c>
+      <c r="L91">
+        <v>0</v>
+      </c>
+      <c r="M91">
+        <v>0</v>
+      </c>
+      <c r="Z91">
+        <v>1</v>
+      </c>
+      <c r="AD91" t="s">
         <v>346</v>
-      </c>
-      <c r="L91">
-        <v>0</v>
-      </c>
-      <c r="M91">
-        <v>0</v>
-      </c>
-      <c r="Z91">
-        <v>1</v>
-      </c>
-      <c r="AD91" t="s">
-        <v>347</v>
       </c>
       <c r="AE91">
         <v>0.5</v>
@@ -10476,25 +10476,25 @@
     </row>
     <row r="92" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D92" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E92" t="s">
         <v>301</v>
       </c>
       <c r="F92" t="s">
+        <v>348</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92">
+        <v>0</v>
+      </c>
+      <c r="Z92">
+        <v>1</v>
+      </c>
+      <c r="AD92" t="s">
         <v>349</v>
-      </c>
-      <c r="L92">
-        <v>0</v>
-      </c>
-      <c r="M92">
-        <v>0</v>
-      </c>
-      <c r="Z92">
-        <v>1</v>
-      </c>
-      <c r="AD92" t="s">
-        <v>350</v>
       </c>
       <c r="AE92">
         <v>0.5</v>
@@ -10553,25 +10553,25 @@
     </row>
     <row r="93" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D93" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E93" t="s">
         <v>301</v>
       </c>
       <c r="F93" t="s">
+        <v>351</v>
+      </c>
+      <c r="L93">
+        <v>0</v>
+      </c>
+      <c r="M93">
+        <v>0</v>
+      </c>
+      <c r="Z93">
+        <v>1</v>
+      </c>
+      <c r="AD93" t="s">
         <v>352</v>
-      </c>
-      <c r="L93">
-        <v>0</v>
-      </c>
-      <c r="M93">
-        <v>0</v>
-      </c>
-      <c r="Z93">
-        <v>1</v>
-      </c>
-      <c r="AD93" t="s">
-        <v>353</v>
       </c>
       <c r="AE93">
         <v>0.5</v>
@@ -10630,25 +10630,25 @@
     </row>
     <row r="94" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D94" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E94" t="s">
         <v>301</v>
       </c>
       <c r="F94" t="s">
+        <v>354</v>
+      </c>
+      <c r="L94">
+        <v>0</v>
+      </c>
+      <c r="M94">
+        <v>0</v>
+      </c>
+      <c r="Z94">
+        <v>1</v>
+      </c>
+      <c r="AD94" t="s">
         <v>355</v>
-      </c>
-      <c r="L94">
-        <v>0</v>
-      </c>
-      <c r="M94">
-        <v>0</v>
-      </c>
-      <c r="Z94">
-        <v>1</v>
-      </c>
-      <c r="AD94" t="s">
-        <v>356</v>
       </c>
       <c r="AE94">
         <v>0.5</v>
@@ -10707,22 +10707,22 @@
     </row>
     <row r="95" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D95" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E95" t="s">
         <v>301</v>
       </c>
       <c r="F95" t="s">
+        <v>357</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95">
+        <v>0</v>
+      </c>
+      <c r="AD95" t="s">
         <v>358</v>
-      </c>
-      <c r="L95">
-        <v>0</v>
-      </c>
-      <c r="M95">
-        <v>0</v>
-      </c>
-      <c r="AD95" t="s">
-        <v>359</v>
       </c>
       <c r="AE95">
         <v>0.5</v>
@@ -10781,13 +10781,13 @@
     </row>
     <row r="96" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D96" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E96" t="s">
         <v>301</v>
       </c>
       <c r="F96" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L96">
         <v>0</v>
@@ -10849,22 +10849,22 @@
     </row>
     <row r="97" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D97" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E97" t="s">
         <v>301</v>
       </c>
       <c r="F97" t="s">
+        <v>362</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97">
+        <v>0</v>
+      </c>
+      <c r="X97" t="s">
         <v>363</v>
-      </c>
-      <c r="L97">
-        <v>0</v>
-      </c>
-      <c r="M97">
-        <v>0</v>
-      </c>
-      <c r="X97" t="s">
-        <v>364</v>
       </c>
       <c r="AF97">
         <v>0</v>
@@ -10917,28 +10917,28 @@
     </row>
     <row r="98" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D98" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E98" t="s">
         <v>301</v>
       </c>
       <c r="F98" t="s">
+        <v>365</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98">
+        <v>0</v>
+      </c>
+      <c r="V98">
+        <v>0</v>
+      </c>
+      <c r="W98">
+        <v>0</v>
+      </c>
+      <c r="AD98" t="s">
         <v>366</v>
-      </c>
-      <c r="L98">
-        <v>0</v>
-      </c>
-      <c r="M98">
-        <v>0</v>
-      </c>
-      <c r="V98">
-        <v>0</v>
-      </c>
-      <c r="W98">
-        <v>0</v>
-      </c>
-      <c r="AD98" t="s">
-        <v>367</v>
       </c>
       <c r="AE98">
         <v>0.45</v>
@@ -10997,28 +10997,28 @@
     </row>
     <row r="99" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D99" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E99" t="s">
         <v>301</v>
       </c>
       <c r="F99" t="s">
+        <v>368</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+      <c r="M99">
+        <v>0</v>
+      </c>
+      <c r="V99">
+        <v>0</v>
+      </c>
+      <c r="W99">
+        <v>0</v>
+      </c>
+      <c r="AD99" t="s">
         <v>369</v>
-      </c>
-      <c r="L99">
-        <v>0</v>
-      </c>
-      <c r="M99">
-        <v>0</v>
-      </c>
-      <c r="V99">
-        <v>0</v>
-      </c>
-      <c r="W99">
-        <v>0</v>
-      </c>
-      <c r="AD99" t="s">
-        <v>370</v>
       </c>
       <c r="AE99">
         <v>0.45</v>
@@ -11077,28 +11077,28 @@
     </row>
     <row r="100" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D100" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E100" t="s">
         <v>301</v>
       </c>
       <c r="F100" t="s">
+        <v>371</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100">
+        <v>0</v>
+      </c>
+      <c r="V100">
+        <v>0</v>
+      </c>
+      <c r="W100">
+        <v>0</v>
+      </c>
+      <c r="X100" t="s">
         <v>372</v>
-      </c>
-      <c r="L100">
-        <v>0</v>
-      </c>
-      <c r="M100">
-        <v>0</v>
-      </c>
-      <c r="V100">
-        <v>0</v>
-      </c>
-      <c r="W100">
-        <v>0</v>
-      </c>
-      <c r="X100" t="s">
-        <v>373</v>
       </c>
       <c r="AF100">
         <v>0</v>
@@ -11151,13 +11151,13 @@
     </row>
     <row r="101" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D101" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E101" t="s">
         <v>301</v>
       </c>
       <c r="F101" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L101">
         <v>0</v>
@@ -11172,7 +11172,7 @@
         <v>0</v>
       </c>
       <c r="X101" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AF101">
         <v>0</v>
@@ -11225,13 +11225,13 @@
     </row>
     <row r="102" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D102" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E102" t="s">
         <v>301</v>
       </c>
       <c r="F102" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L102">
         <v>0</v>
@@ -11246,7 +11246,7 @@
         <v>0</v>
       </c>
       <c r="X102" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AF102">
         <v>0</v>
@@ -11299,13 +11299,13 @@
     </row>
     <row r="103" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D103" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E103" t="s">
         <v>301</v>
       </c>
       <c r="F103" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L103">
         <v>0</v>
@@ -11320,7 +11320,7 @@
         <v>0</v>
       </c>
       <c r="X103" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AF103">
         <v>0</v>
@@ -11373,13 +11373,13 @@
     </row>
     <row r="104" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D104" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E104" t="s">
         <v>301</v>
       </c>
       <c r="F104" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="L104">
         <v>0</v>
@@ -11444,28 +11444,28 @@
     </row>
     <row r="105" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D105" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E105" t="s">
         <v>301</v>
       </c>
       <c r="F105" t="s">
+        <v>382</v>
+      </c>
+      <c r="L105">
+        <v>0</v>
+      </c>
+      <c r="M105">
+        <v>0</v>
+      </c>
+      <c r="V105">
+        <v>0</v>
+      </c>
+      <c r="W105">
+        <v>0</v>
+      </c>
+      <c r="X105" t="s">
         <v>383</v>
-      </c>
-      <c r="L105">
-        <v>0</v>
-      </c>
-      <c r="M105">
-        <v>0</v>
-      </c>
-      <c r="V105">
-        <v>0</v>
-      </c>
-      <c r="W105">
-        <v>0</v>
-      </c>
-      <c r="X105" t="s">
-        <v>384</v>
       </c>
       <c r="AF105">
         <v>0</v>
@@ -11518,28 +11518,28 @@
     </row>
     <row r="106" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D106" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E106" t="s">
         <v>301</v>
       </c>
       <c r="F106" t="s">
+        <v>385</v>
+      </c>
+      <c r="L106">
+        <v>0</v>
+      </c>
+      <c r="M106">
+        <v>0</v>
+      </c>
+      <c r="V106">
+        <v>0</v>
+      </c>
+      <c r="W106">
+        <v>0</v>
+      </c>
+      <c r="X106" t="s">
         <v>386</v>
-      </c>
-      <c r="L106">
-        <v>0</v>
-      </c>
-      <c r="M106">
-        <v>0</v>
-      </c>
-      <c r="V106">
-        <v>0</v>
-      </c>
-      <c r="W106">
-        <v>0</v>
-      </c>
-      <c r="X106" t="s">
-        <v>387</v>
       </c>
       <c r="AF106">
         <v>0</v>
@@ -11592,19 +11592,19 @@
     </row>
     <row r="107" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D107" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E107" t="s">
         <v>301</v>
       </c>
       <c r="F107" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Z107">
         <v>1</v>
       </c>
       <c r="AD107" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AE107">
         <v>0.15</v>
@@ -11663,19 +11663,19 @@
     </row>
     <row r="108" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D108" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E108" t="s">
         <v>301</v>
       </c>
       <c r="F108" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="Z108">
         <v>1</v>
       </c>
       <c r="AD108" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AE108">
         <v>0.15</v>
@@ -11734,16 +11734,16 @@
     </row>
     <row r="109" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D109" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E109" t="s">
         <v>301</v>
       </c>
       <c r="F109" t="s">
+        <v>392</v>
+      </c>
+      <c r="X109" t="s">
         <v>393</v>
-      </c>
-      <c r="X109" t="s">
-        <v>394</v>
       </c>
       <c r="Z109">
         <v>1</v>
@@ -11799,19 +11799,19 @@
     </row>
     <row r="110" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D110" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E110" t="s">
         <v>301</v>
       </c>
       <c r="F110" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Z110">
         <v>1</v>
       </c>
       <c r="AD110" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AE110">
         <v>0.15</v>
@@ -11870,19 +11870,19 @@
     </row>
     <row r="111" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D111" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E111" t="s">
         <v>301</v>
       </c>
       <c r="F111" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Z111">
         <v>1</v>
       </c>
       <c r="AD111" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AE111">
         <v>0.15</v>
@@ -11941,19 +11941,19 @@
     </row>
     <row r="112" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D112" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E112" t="s">
         <v>301</v>
       </c>
       <c r="F112" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Z112">
         <v>1</v>
       </c>
       <c r="AD112" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AE112">
         <v>0.15</v>
@@ -12012,19 +12012,19 @@
     </row>
     <row r="113" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D113" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E113" t="s">
         <v>301</v>
       </c>
       <c r="F113" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Z113">
         <v>1</v>
       </c>
       <c r="AD113" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AE113">
         <v>0.15</v>
@@ -12083,39 +12083,39 @@
     </row>
     <row r="114" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D114" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E114" t="s">
         <v>301</v>
       </c>
       <c r="F114" t="s">
+        <v>437</v>
+      </c>
+      <c r="L114">
+        <v>0</v>
+      </c>
+      <c r="M114">
+        <v>0</v>
+      </c>
+      <c r="V114">
+        <v>0</v>
+      </c>
+      <c r="W114">
+        <v>0</v>
+      </c>
+      <c r="X114" t="s">
         <v>438</v>
-      </c>
-      <c r="L114">
-        <v>0</v>
-      </c>
-      <c r="M114">
-        <v>0</v>
-      </c>
-      <c r="V114">
-        <v>0</v>
-      </c>
-      <c r="W114">
-        <v>0</v>
-      </c>
-      <c r="X114" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="115" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D115" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E115" t="s">
         <v>301</v>
       </c>
       <c r="F115" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L115">
         <v>0</v>
@@ -12132,13 +12132,13 @@
     </row>
     <row r="116" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D116" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E116" t="s">
         <v>301</v>
       </c>
       <c r="F116" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="L116">
         <v>0</v>
@@ -12203,13 +12203,13 @@
     </row>
     <row r="117" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D117" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E117" t="s">
         <v>301</v>
       </c>
       <c r="F117" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="L117">
         <v>0</v>
@@ -12274,28 +12274,28 @@
     </row>
     <row r="118" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D118" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E118" t="s">
         <v>301</v>
       </c>
       <c r="F118" t="s">
+        <v>430</v>
+      </c>
+      <c r="L118">
+        <v>0</v>
+      </c>
+      <c r="M118">
+        <v>0</v>
+      </c>
+      <c r="V118">
+        <v>0</v>
+      </c>
+      <c r="W118">
+        <v>0</v>
+      </c>
+      <c r="X118" t="s">
         <v>431</v>
-      </c>
-      <c r="L118">
-        <v>0</v>
-      </c>
-      <c r="M118">
-        <v>0</v>
-      </c>
-      <c r="V118">
-        <v>0</v>
-      </c>
-      <c r="W118">
-        <v>0</v>
-      </c>
-      <c r="X118" t="s">
-        <v>432</v>
       </c>
       <c r="AF118">
         <v>0</v>
@@ -12348,13 +12348,13 @@
     </row>
     <row r="119" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D119" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E119" t="s">
         <v>301</v>
       </c>
       <c r="F119" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="L119">
         <v>0</v>
@@ -12417,18 +12417,18 @@
         <v>0</v>
       </c>
       <c r="BD119" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="120" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D120" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E120" t="s">
         <v>301</v>
       </c>
       <c r="F120" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L120">
         <v>0</v>
@@ -12496,13 +12496,13 @@
     </row>
     <row r="121" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D121" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E121" t="s">
         <v>301</v>
       </c>
       <c r="F121" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L121">
         <v>0</v>
@@ -12567,13 +12567,13 @@
     </row>
     <row r="122" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D122" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E122" t="s">
         <v>301</v>
       </c>
       <c r="F122" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L122">
         <v>0</v>
@@ -12641,28 +12641,28 @@
     </row>
     <row r="123" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D123" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E123" t="s">
         <v>301</v>
       </c>
       <c r="F123" t="s">
+        <v>419</v>
+      </c>
+      <c r="L123">
+        <v>0</v>
+      </c>
+      <c r="M123">
+        <v>0</v>
+      </c>
+      <c r="V123">
+        <v>0</v>
+      </c>
+      <c r="W123">
+        <v>0</v>
+      </c>
+      <c r="X123" t="s">
         <v>420</v>
-      </c>
-      <c r="L123">
-        <v>0</v>
-      </c>
-      <c r="M123">
-        <v>0</v>
-      </c>
-      <c r="V123">
-        <v>0</v>
-      </c>
-      <c r="W123">
-        <v>0</v>
-      </c>
-      <c r="X123" t="s">
-        <v>421</v>
       </c>
       <c r="AF123">
         <v>0</v>
@@ -12706,102 +12706,102 @@
     </row>
     <row r="124" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D124" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E124" t="s">
         <v>301</v>
       </c>
       <c r="F124" t="s">
+        <v>417</v>
+      </c>
+      <c r="L124">
+        <v>0</v>
+      </c>
+      <c r="M124">
+        <v>0</v>
+      </c>
+      <c r="V124">
+        <v>0</v>
+      </c>
+      <c r="W124">
+        <v>0</v>
+      </c>
+      <c r="AF124">
+        <v>0</v>
+      </c>
+      <c r="AG124">
+        <v>0</v>
+      </c>
+      <c r="AH124">
+        <v>0</v>
+      </c>
+      <c r="AI124">
+        <v>0</v>
+      </c>
+      <c r="AJ124">
+        <v>0</v>
+      </c>
+      <c r="AO124">
+        <v>0</v>
+      </c>
+      <c r="AR124">
+        <v>0</v>
+      </c>
+      <c r="AT124">
+        <v>0</v>
+      </c>
+      <c r="AU124">
+        <v>0</v>
+      </c>
+      <c r="AW124">
+        <v>0</v>
+      </c>
+      <c r="AX124">
+        <v>0</v>
+      </c>
+      <c r="AY124">
+        <v>0</v>
+      </c>
+      <c r="AZ124">
+        <v>0</v>
+      </c>
+      <c r="BA124">
+        <v>0</v>
+      </c>
+      <c r="BB124">
+        <v>0</v>
+      </c>
+      <c r="BC124">
+        <v>0</v>
+      </c>
+      <c r="BD124" t="s">
         <v>418</v>
-      </c>
-      <c r="L124">
-        <v>0</v>
-      </c>
-      <c r="M124">
-        <v>0</v>
-      </c>
-      <c r="V124">
-        <v>0</v>
-      </c>
-      <c r="W124">
-        <v>0</v>
-      </c>
-      <c r="AF124">
-        <v>0</v>
-      </c>
-      <c r="AG124">
-        <v>0</v>
-      </c>
-      <c r="AH124">
-        <v>0</v>
-      </c>
-      <c r="AI124">
-        <v>0</v>
-      </c>
-      <c r="AJ124">
-        <v>0</v>
-      </c>
-      <c r="AO124">
-        <v>0</v>
-      </c>
-      <c r="AR124">
-        <v>0</v>
-      </c>
-      <c r="AT124">
-        <v>0</v>
-      </c>
-      <c r="AU124">
-        <v>0</v>
-      </c>
-      <c r="AW124">
-        <v>0</v>
-      </c>
-      <c r="AX124">
-        <v>0</v>
-      </c>
-      <c r="AY124">
-        <v>0</v>
-      </c>
-      <c r="AZ124">
-        <v>0</v>
-      </c>
-      <c r="BA124">
-        <v>0</v>
-      </c>
-      <c r="BB124">
-        <v>0</v>
-      </c>
-      <c r="BC124">
-        <v>0</v>
-      </c>
-      <c r="BD124" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="125" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D125" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E125" t="s">
         <v>301</v>
       </c>
       <c r="F125" t="s">
+        <v>414</v>
+      </c>
+      <c r="L125">
+        <v>0</v>
+      </c>
+      <c r="M125">
+        <v>0</v>
+      </c>
+      <c r="V125">
+        <v>0</v>
+      </c>
+      <c r="W125">
+        <v>0</v>
+      </c>
+      <c r="AD125" t="s">
         <v>415</v>
-      </c>
-      <c r="L125">
-        <v>0</v>
-      </c>
-      <c r="M125">
-        <v>0</v>
-      </c>
-      <c r="V125">
-        <v>0</v>
-      </c>
-      <c r="W125">
-        <v>0</v>
-      </c>
-      <c r="AD125" t="s">
-        <v>416</v>
       </c>
       <c r="AE125">
         <v>0.25</v>
@@ -12863,28 +12863,28 @@
     </row>
     <row r="126" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D126" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E126" t="s">
         <v>301</v>
       </c>
       <c r="F126" t="s">
+        <v>411</v>
+      </c>
+      <c r="L126">
+        <v>0</v>
+      </c>
+      <c r="M126">
+        <v>0</v>
+      </c>
+      <c r="V126">
+        <v>0</v>
+      </c>
+      <c r="W126">
+        <v>0</v>
+      </c>
+      <c r="AD126" t="s">
         <v>412</v>
-      </c>
-      <c r="L126">
-        <v>0</v>
-      </c>
-      <c r="M126">
-        <v>0</v>
-      </c>
-      <c r="V126">
-        <v>0</v>
-      </c>
-      <c r="W126">
-        <v>0</v>
-      </c>
-      <c r="AD126" t="s">
-        <v>413</v>
       </c>
       <c r="AE126">
         <v>0.75</v>
@@ -12946,13 +12946,13 @@
     </row>
     <row r="127" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D127" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E127" t="s">
         <v>301</v>
       </c>
       <c r="F127" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="L127">
         <v>0</v>
@@ -13017,28 +13017,28 @@
     </row>
     <row r="128" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D128" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E128" t="s">
         <v>301</v>
       </c>
       <c r="F128" t="s">
+        <v>406</v>
+      </c>
+      <c r="L128">
+        <v>0</v>
+      </c>
+      <c r="M128">
+        <v>0</v>
+      </c>
+      <c r="V128">
+        <v>0</v>
+      </c>
+      <c r="W128">
+        <v>0</v>
+      </c>
+      <c r="AD128" t="s">
         <v>407</v>
-      </c>
-      <c r="L128">
-        <v>0</v>
-      </c>
-      <c r="M128">
-        <v>0</v>
-      </c>
-      <c r="V128">
-        <v>0</v>
-      </c>
-      <c r="W128">
-        <v>0</v>
-      </c>
-      <c r="AD128" t="s">
-        <v>408</v>
       </c>
       <c r="AE128">
         <v>0.75</v>
@@ -13097,28 +13097,28 @@
     </row>
     <row r="129" spans="3:56" x14ac:dyDescent="0.2">
       <c r="D129" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E129" t="s">
         <v>301</v>
       </c>
       <c r="F129" t="s">
+        <v>403</v>
+      </c>
+      <c r="L129">
+        <v>0</v>
+      </c>
+      <c r="M129">
+        <v>0</v>
+      </c>
+      <c r="V129">
+        <v>0</v>
+      </c>
+      <c r="W129">
+        <v>0</v>
+      </c>
+      <c r="X129" t="s">
         <v>404</v>
-      </c>
-      <c r="L129">
-        <v>0</v>
-      </c>
-      <c r="M129">
-        <v>0</v>
-      </c>
-      <c r="V129">
-        <v>0</v>
-      </c>
-      <c r="W129">
-        <v>0</v>
-      </c>
-      <c r="X129" t="s">
-        <v>405</v>
       </c>
       <c r="AF129">
         <v>0</v>

</xml_diff>

<commit_message>
Lots of little and minor fixes, tweaks and changes.
- We can now merge duplicate units for kingdoms.
</commit_message>
<xml_diff>
--- a/resources/data-imports/items-second-set.xlsx
+++ b/resources/data-imports/items-second-set.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A855B028-1601-1A4F-9E97-16EF865EA42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CAB2B2-77A8-DD48-BC31-A3C2A993AD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1278,9 +1278,6 @@
     <t>A simple bag of child's bones. You can give these to Shade Lord for an item.</t>
   </si>
   <si>
-    <t>Lust for Gold</t>
-  </si>
-  <si>
     <t>Purse of Shards and Dust</t>
   </si>
   <si>
@@ -1360,6 +1357,9 @@
   </si>
   <si>
     <t>River Styx Sandals</t>
+  </si>
+  <si>
+    <t>Kingmanship</t>
   </si>
 </sst>
 </file>
@@ -1708,8 +1708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT134" workbookViewId="0">
-      <selection activeCell="D179" sqref="D179"/>
+    <sheetView tabSelected="1" topLeftCell="T83" workbookViewId="0">
+      <selection activeCell="AD125" sqref="AD125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9979,7 +9979,7 @@
     </row>
     <row r="85" spans="4:55" x14ac:dyDescent="0.2">
       <c r="D85" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E85" t="s">
         <v>301</v>
@@ -12083,39 +12083,39 @@
     </row>
     <row r="114" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D114" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E114" t="s">
         <v>301</v>
       </c>
       <c r="F114" t="s">
+        <v>436</v>
+      </c>
+      <c r="L114">
+        <v>0</v>
+      </c>
+      <c r="M114">
+        <v>0</v>
+      </c>
+      <c r="V114">
+        <v>0</v>
+      </c>
+      <c r="W114">
+        <v>0</v>
+      </c>
+      <c r="X114" t="s">
         <v>437</v>
-      </c>
-      <c r="L114">
-        <v>0</v>
-      </c>
-      <c r="M114">
-        <v>0</v>
-      </c>
-      <c r="V114">
-        <v>0</v>
-      </c>
-      <c r="W114">
-        <v>0</v>
-      </c>
-      <c r="X114" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="115" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D115" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E115" t="s">
         <v>301</v>
       </c>
       <c r="F115" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="L115">
         <v>0</v>
@@ -12132,13 +12132,13 @@
     </row>
     <row r="116" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D116" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E116" t="s">
         <v>301</v>
       </c>
       <c r="F116" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="L116">
         <v>0</v>
@@ -12203,13 +12203,13 @@
     </row>
     <row r="117" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D117" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E117" t="s">
         <v>301</v>
       </c>
       <c r="F117" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="L117">
         <v>0</v>
@@ -12274,28 +12274,28 @@
     </row>
     <row r="118" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D118" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E118" t="s">
         <v>301</v>
       </c>
       <c r="F118" t="s">
+        <v>429</v>
+      </c>
+      <c r="L118">
+        <v>0</v>
+      </c>
+      <c r="M118">
+        <v>0</v>
+      </c>
+      <c r="V118">
+        <v>0</v>
+      </c>
+      <c r="W118">
+        <v>0</v>
+      </c>
+      <c r="X118" t="s">
         <v>430</v>
-      </c>
-      <c r="L118">
-        <v>0</v>
-      </c>
-      <c r="M118">
-        <v>0</v>
-      </c>
-      <c r="V118">
-        <v>0</v>
-      </c>
-      <c r="W118">
-        <v>0</v>
-      </c>
-      <c r="X118" t="s">
-        <v>431</v>
       </c>
       <c r="AF118">
         <v>0</v>
@@ -12348,13 +12348,13 @@
     </row>
     <row r="119" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D119" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E119" t="s">
         <v>301</v>
       </c>
       <c r="F119" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L119">
         <v>0</v>
@@ -12417,18 +12417,18 @@
         <v>0</v>
       </c>
       <c r="BD119" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="120" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D120" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E120" t="s">
         <v>301</v>
       </c>
       <c r="F120" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L120">
         <v>0</v>
@@ -12496,13 +12496,13 @@
     </row>
     <row r="121" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D121" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E121" t="s">
         <v>301</v>
       </c>
       <c r="F121" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L121">
         <v>0</v>
@@ -12567,13 +12567,13 @@
     </row>
     <row r="122" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D122" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E122" t="s">
         <v>301</v>
       </c>
       <c r="F122" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="L122">
         <v>0</v>
@@ -12641,28 +12641,28 @@
     </row>
     <row r="123" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D123" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E123" t="s">
         <v>301</v>
       </c>
       <c r="F123" t="s">
+        <v>418</v>
+      </c>
+      <c r="L123">
+        <v>0</v>
+      </c>
+      <c r="M123">
+        <v>0</v>
+      </c>
+      <c r="V123">
+        <v>0</v>
+      </c>
+      <c r="W123">
+        <v>0</v>
+      </c>
+      <c r="X123" t="s">
         <v>419</v>
-      </c>
-      <c r="L123">
-        <v>0</v>
-      </c>
-      <c r="M123">
-        <v>0</v>
-      </c>
-      <c r="V123">
-        <v>0</v>
-      </c>
-      <c r="W123">
-        <v>0</v>
-      </c>
-      <c r="X123" t="s">
-        <v>420</v>
       </c>
       <c r="AF123">
         <v>0</v>
@@ -12706,76 +12706,76 @@
     </row>
     <row r="124" spans="4:56" x14ac:dyDescent="0.2">
       <c r="D124" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E124" t="s">
         <v>301</v>
       </c>
       <c r="F124" t="s">
+        <v>416</v>
+      </c>
+      <c r="L124">
+        <v>0</v>
+      </c>
+      <c r="M124">
+        <v>0</v>
+      </c>
+      <c r="V124">
+        <v>0</v>
+      </c>
+      <c r="W124">
+        <v>0</v>
+      </c>
+      <c r="AF124">
+        <v>0</v>
+      </c>
+      <c r="AG124">
+        <v>0</v>
+      </c>
+      <c r="AH124">
+        <v>0</v>
+      </c>
+      <c r="AI124">
+        <v>0</v>
+      </c>
+      <c r="AJ124">
+        <v>0</v>
+      </c>
+      <c r="AO124">
+        <v>0</v>
+      </c>
+      <c r="AR124">
+        <v>0</v>
+      </c>
+      <c r="AT124">
+        <v>0</v>
+      </c>
+      <c r="AU124">
+        <v>0</v>
+      </c>
+      <c r="AW124">
+        <v>0</v>
+      </c>
+      <c r="AX124">
+        <v>0</v>
+      </c>
+      <c r="AY124">
+        <v>0</v>
+      </c>
+      <c r="AZ124">
+        <v>0</v>
+      </c>
+      <c r="BA124">
+        <v>0</v>
+      </c>
+      <c r="BB124">
+        <v>0</v>
+      </c>
+      <c r="BC124">
+        <v>0</v>
+      </c>
+      <c r="BD124" t="s">
         <v>417</v>
-      </c>
-      <c r="L124">
-        <v>0</v>
-      </c>
-      <c r="M124">
-        <v>0</v>
-      </c>
-      <c r="V124">
-        <v>0</v>
-      </c>
-      <c r="W124">
-        <v>0</v>
-      </c>
-      <c r="AF124">
-        <v>0</v>
-      </c>
-      <c r="AG124">
-        <v>0</v>
-      </c>
-      <c r="AH124">
-        <v>0</v>
-      </c>
-      <c r="AI124">
-        <v>0</v>
-      </c>
-      <c r="AJ124">
-        <v>0</v>
-      </c>
-      <c r="AO124">
-        <v>0</v>
-      </c>
-      <c r="AR124">
-        <v>0</v>
-      </c>
-      <c r="AT124">
-        <v>0</v>
-      </c>
-      <c r="AU124">
-        <v>0</v>
-      </c>
-      <c r="AW124">
-        <v>0</v>
-      </c>
-      <c r="AX124">
-        <v>0</v>
-      </c>
-      <c r="AY124">
-        <v>0</v>
-      </c>
-      <c r="AZ124">
-        <v>0</v>
-      </c>
-      <c r="BA124">
-        <v>0</v>
-      </c>
-      <c r="BB124">
-        <v>0</v>
-      </c>
-      <c r="BC124">
-        <v>0</v>
-      </c>
-      <c r="BD124" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="125" spans="4:56" x14ac:dyDescent="0.2">
@@ -12801,7 +12801,7 @@
         <v>0</v>
       </c>
       <c r="AD125" t="s">
-        <v>415</v>
+        <v>442</v>
       </c>
       <c r="AE125">
         <v>0.25</v>

</xml_diff>

<commit_message>
Fixes and changes. Updates to the documentation.
</commit_message>
<xml_diff>
--- a/resources/data-imports/items-second-set.xlsx
+++ b/resources/data-imports/items-second-set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CAB2B2-77A8-DD48-BC31-A3C2A993AD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976C5CEE-D30F-6442-A6B4-C29FDBD2978C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -1708,8 +1708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T83" workbookViewId="0">
-      <selection activeCell="AD125" sqref="AD125"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="BD128" sqref="BD128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11220,7 +11220,7 @@
         <v>0.5</v>
       </c>
       <c r="BC101">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="102" spans="4:55" x14ac:dyDescent="0.2">
@@ -11294,7 +11294,7 @@
         <v>0.75</v>
       </c>
       <c r="BC102">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="103" spans="4:55" x14ac:dyDescent="0.2">
@@ -11368,7 +11368,7 @@
         <v>1</v>
       </c>
       <c r="BC103">
-        <v>0.85</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="4:55" x14ac:dyDescent="0.2">
@@ -13089,10 +13089,10 @@
         <v>0</v>
       </c>
       <c r="BB128">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="BC128">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="129" spans="3:56" x14ac:dyDescent="0.2">
@@ -13163,10 +13163,10 @@
         <v>0</v>
       </c>
       <c r="BB129">
-        <v>1</v>
+        <v>0.45</v>
       </c>
       <c r="BC129">
-        <v>1</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="130" spans="3:56" x14ac:dyDescent="0.2">

</xml_diff>